<commit_message>
Test case successful for unicode and special characters
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t xml:space="preserve">Enter a postal code example 10005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TU05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response when passing a city name with unicode in it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weather São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a city with special character like São Paulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converted to plain alphabet and then pushed to array</t>
   </si>
 </sst>
 </file>
@@ -101,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -131,6 +146,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -142,8 +163,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFAA61A"/>
-        <bgColor rgb="FFFFCC00"/>
+        <fgColor rgb="FFF7A19A"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -195,7 +216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,11 +241,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,14 +305,14 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFAA61A"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -308,7 +337,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,7 +451,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Test case for unknown city
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -107,6 +107,36 @@
   </si>
   <si>
     <t xml:space="preserve">Converted to plain alphabet and then pushed to array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TU06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response if Pluto is given in argument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weather Pluto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a city name Pluto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As expected because Pluto is a city in MS, USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TU07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response if Jupitor planet is given in the argument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weather Jupitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As per weather API, result should be 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As expected because Jupitor is a planet and not a city, no data available</t>
   </si>
 </sst>
 </file>
@@ -116,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,12 +176,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -241,20 +265,20 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -337,7 +361,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,47 +456,85 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Test case for all array elements
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t xml:space="preserve">Test Case ID</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t xml:space="preserve">As expected because Jupitor is a planet and not a city, no data available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TU08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response when passing all previous test cases in an array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./weather New York, 10005, Tokyo, São Paulo, Pluto, Juptior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter all the previous arguments in array</t>
   </si>
 </sst>
 </file>
@@ -146,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -177,19 +189,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF7A19A"/>
-        <bgColor rgb="FFFF8080"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -240,7 +252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,11 +277,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,6 +291,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -290,66 +310,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFF7A19A"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -361,7 +321,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -535,7 +495,26 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>